<commit_message>
make several changes to 04, 01
</commit_message>
<xml_diff>
--- a/data_out/Original_Areas_Crops.xlsx
+++ b/data_out/Original_Areas_Crops.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/paulukonis_elizabeth_epa_gov/Documents/Profile/Documents/GitHub/probabilistic_crop_McCaffrey/data_out/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="8_{05282096-E045-4406-B37A-E2886A0F60A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CFD08C9E-4AC0-4464-B2EB-72BAF6DB9F74}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="8_{05282096-E045-4406-B37A-E2886A0F60A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0B7B720D-0BA1-456F-BB9B-A6B5E89F53A2}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E3CB831F-CCE0-4A7F-B7F2-731A4BFC8ED7}"/>
   </bookViews>
@@ -212,16 +212,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{757D2B07-7936-4A6E-8B2D-F99A6B86A1AB}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -555,32 +555,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1165,22 +1165,22 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="2">
         <v>154539.1</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="2">
         <v>270396.79999999999</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="2">
         <v>124982.8</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32" s="2">
         <v>197224.3</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F32" s="2">
         <v>232515</v>
       </c>
     </row>

</xml_diff>